<commit_message>
data till 6 Mar 10AM
</commit_message>
<xml_diff>
--- a/JioMobile/March2021Mobile.xlsx
+++ b/JioMobile/March2021Mobile.xlsx
@@ -70,6 +70,52 @@
         </r>
       </text>
     </comment>
+    <comment ref="M46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+4000-Digital
+1000-Cash</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M49" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+4300-Digital
+200-Cash</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -613,10 +659,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
@@ -636,24 +682,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -661,99 +692,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,18 +712,126 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -860,19 +906,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,25 +930,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,7 +954,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,49 +1044,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -986,25 +1062,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1017,18 +1075,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1063,11 +1109,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1081,17 +1144,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1111,51 +1183,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1165,13 +1211,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1183,130 +1229,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1757,11 +1803,11 @@
   <dimension ref="A1:AT114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="J36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L49" sqref="L49"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1909,26 +1955,26 @@
       <c r="A2" s="13"/>
       <c r="B2" s="24">
         <f>SUM(F3:F121)</f>
-        <v>225000</v>
+        <v>250500</v>
       </c>
       <c r="D2" s="14">
         <f>SUM(H3:H121)</f>
-        <v>225000</v>
+        <v>250500</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="25">
         <f>H2+I2</f>
-        <v>225000</v>
+        <v>250500</v>
       </c>
       <c r="G2" s="25">
         <f>H2/1500</f>
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="H2" s="14">
         <f>SUM(J2:AN2)</f>
-        <v>225000</v>
+        <v>250500</v>
       </c>
       <c r="I2" s="32">
         <f>SUM(I3:I121)</f>
@@ -1948,11 +1994,11 @@
       </c>
       <c r="M2" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="N2" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19500</v>
       </c>
       <c r="O2" s="10">
         <f t="shared" si="0"/>
@@ -2138,7 +2184,7 @@
       </c>
       <c r="I5" s="33"/>
     </row>
-    <row r="6" s="11" customFormat="1" spans="1:11">
+    <row r="6" s="11" customFormat="1" spans="1:13">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -2153,20 +2199,24 @@
       </c>
       <c r="F6" s="10">
         <f t="shared" si="1"/>
-        <v>7500</v>
+        <v>13500</v>
       </c>
       <c r="G6" s="10">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H6" s="10">
         <f t="shared" si="3"/>
-        <v>7500</v>
+        <v>13500</v>
       </c>
       <c r="I6" s="33"/>
       <c r="K6" s="11">
         <f>5*1500</f>
         <v>7500</v>
+      </c>
+      <c r="M6" s="11">
+        <f>4*1500</f>
+        <v>6000</v>
       </c>
     </row>
     <row r="7" s="11" customFormat="1" spans="1:9">
@@ -2537,7 +2587,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="20" s="11" customFormat="1" spans="1:9">
+    <row r="20" s="11" customFormat="1" spans="1:14">
       <c r="A20" s="11">
         <v>18</v>
       </c>
@@ -2549,17 +2599,21 @@
       </c>
       <c r="F20" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G20" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I20" s="33"/>
+      <c r="N20" s="11">
+        <f>2*1500</f>
+        <v>3000</v>
+      </c>
     </row>
     <row r="21" s="11" customFormat="1" spans="1:12">
       <c r="A21" s="11">
@@ -3292,7 +3346,7 @@
       </c>
       <c r="I48" s="33"/>
     </row>
-    <row r="49" s="11" customFormat="1" spans="1:12">
+    <row r="49" s="11" customFormat="1" spans="1:14">
       <c r="A49" s="11">
         <v>47</v>
       </c>
@@ -3304,21 +3358,25 @@
       </c>
       <c r="F49" s="10">
         <f t="shared" si="4"/>
-        <v>3000</v>
+        <v>7500</v>
       </c>
       <c r="G49" s="10">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H49" s="10">
         <f t="shared" si="6"/>
-        <v>3000</v>
+        <v>7500</v>
       </c>
       <c r="I49" s="33"/>
       <c r="L49" s="11">
         <f>2*1500</f>
         <v>3000</v>
       </c>
+      <c r="N49" s="11">
+        <f>3*1500</f>
+        <v>4500</v>
+      </c>
     </row>
     <row r="50" s="11" customFormat="1" spans="1:9">
       <c r="A50" s="11">
@@ -3372,7 +3430,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="52" s="11" customFormat="1" spans="1:9">
+    <row r="52" s="11" customFormat="1" spans="1:14">
       <c r="A52" s="11">
         <v>50</v>
       </c>
@@ -3384,17 +3442,21 @@
       </c>
       <c r="F52" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="G52" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H52" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="I52" s="33"/>
+      <c r="N52" s="11">
+        <f>3*1500</f>
+        <v>4500</v>
+      </c>
     </row>
     <row r="53" s="11" customFormat="1" spans="1:12">
       <c r="A53" s="11">
@@ -3885,7 +3947,7 @@
       </c>
       <c r="I71" s="33"/>
     </row>
-    <row r="72" s="11" customFormat="1" spans="1:9">
+    <row r="72" s="11" customFormat="1" spans="1:14">
       <c r="A72" s="11">
         <v>70</v>
       </c>
@@ -3897,17 +3959,21 @@
       </c>
       <c r="F72" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>7500</v>
       </c>
       <c r="G72" s="10">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H72" s="10">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>7500</v>
       </c>
       <c r="I72" s="33"/>
+      <c r="N72" s="11">
+        <f>5*1500</f>
+        <v>7500</v>
+      </c>
     </row>
     <row r="73" s="11" customFormat="1" spans="1:12">
       <c r="A73" s="11">
@@ -4625,7 +4691,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K50" sqref="K50"/>
+      <selection pane="bottomRight" activeCell="M101" sqref="M101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -4773,14 +4839,14 @@
       <c r="E2" s="13"/>
       <c r="F2" s="14">
         <f>SUM(H3:H121)</f>
-        <v>194500</v>
+        <v>222000</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="16">
         <f>SUM(I2:AM2)</f>
-        <v>194500</v>
+        <v>222000</v>
       </c>
       <c r="I2" s="10">
         <f t="shared" ref="I2:AB2" si="0">SUM(I3:I121)</f>
@@ -4796,11 +4862,11 @@
       </c>
       <c r="L2" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="M2" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21500</v>
       </c>
       <c r="N2" s="10">
         <f t="shared" si="0"/>
@@ -5012,10 +5078,13 @@
       </c>
       <c r="H6" s="10">
         <f t="shared" si="2"/>
-        <v>7500</v>
+        <v>13500</v>
       </c>
       <c r="J6" s="11">
         <v>7500</v>
+      </c>
+      <c r="L6" s="11">
+        <v>6000</v>
       </c>
       <c r="AB6" s="21"/>
     </row>
@@ -5991,10 +6060,13 @@
       </c>
       <c r="H46" s="10">
         <f t="shared" si="3"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="K46" s="11">
         <v>10000</v>
+      </c>
+      <c r="M46" s="19">
+        <v>5000</v>
       </c>
       <c r="AB46" s="21"/>
     </row>
@@ -6069,10 +6141,13 @@
       </c>
       <c r="H49" s="10">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>7500</v>
       </c>
       <c r="K49" s="11">
         <v>3000</v>
+      </c>
+      <c r="M49" s="19">
+        <v>4500</v>
       </c>
       <c r="AB49" s="21"/>
     </row>
@@ -6147,7 +6222,10 @@
       </c>
       <c r="H52" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4500</v>
+      </c>
+      <c r="M52" s="11">
+        <v>4500</v>
       </c>
       <c r="AB52" s="21"/>
     </row>
@@ -6605,7 +6683,10 @@
       </c>
       <c r="H72" s="10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7500</v>
+      </c>
+      <c r="M72" s="11">
+        <v>7500</v>
       </c>
       <c r="AB72" s="21"/>
     </row>
@@ -7174,7 +7255,7 @@
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D59" sqref="A1:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -7210,7 +7291,7 @@
       </c>
       <c r="D2" s="6">
         <f>Orders!F2-Collection!H2</f>
-        <v>30500</v>
+        <v>28500</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -7476,7 +7557,7 @@
       </c>
       <c r="D20" s="9">
         <f>Orders!F20-Collection!H20</f>
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -7862,7 +7943,7 @@
       </c>
       <c r="D46" s="9">
         <f>Orders!F46-Collection!H46</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -8562,6 +8643,9 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D96">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
data till 7 Mar 11AM
</commit_message>
<xml_diff>
--- a/JioMobile/March2021Mobile.xlsx
+++ b/JioMobile/March2021Mobile.xlsx
@@ -659,11 +659,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -682,16 +682,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -705,60 +704,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -772,8 +718,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -781,17 +728,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -804,7 +750,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -820,18 +766,72 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -906,7 +906,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,25 +948,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -972,12 +1020,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -990,7 +1032,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1002,7 +1050,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1014,73 +1080,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1126,20 +1126,35 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1155,15 +1170,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1192,17 +1198,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1211,13 +1211,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1229,40 +1229,40 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1271,88 +1271,88 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1803,11 +1803,11 @@
   <dimension ref="A1:AT114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1955,26 +1955,26 @@
       <c r="A2" s="13"/>
       <c r="B2" s="24">
         <f>SUM(F3:F121)</f>
-        <v>250500</v>
+        <v>256500</v>
       </c>
       <c r="D2" s="14">
         <f>SUM(H3:H121)</f>
-        <v>250500</v>
+        <v>256500</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="25">
         <f>H2+I2</f>
-        <v>250500</v>
+        <v>256500</v>
       </c>
       <c r="G2" s="25">
         <f>H2/1500</f>
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="H2" s="14">
         <f>SUM(J2:AN2)</f>
-        <v>250500</v>
+        <v>256500</v>
       </c>
       <c r="I2" s="32">
         <f>SUM(I3:I121)</f>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="O2" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="P2" s="10">
         <f t="shared" si="0"/>
@@ -2332,7 +2332,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="11" s="11" customFormat="1" spans="1:9">
+    <row r="11" s="11" customFormat="1" spans="1:15">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -2344,17 +2344,21 @@
       </c>
       <c r="F11" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G11" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H11" s="10">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="I11" s="33"/>
+      <c r="O11" s="11">
+        <f>4*1500</f>
+        <v>6000</v>
+      </c>
     </row>
     <row r="12" s="11" customFormat="1" spans="1:9">
       <c r="A12" s="11">
@@ -4687,11 +4691,11 @@
   <dimension ref="A1:AM112"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="I36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="I89" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M101" sqref="M101"/>
+      <selection pane="bottomRight" activeCell="N89" sqref="N89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -4839,14 +4843,14 @@
       <c r="E2" s="13"/>
       <c r="F2" s="14">
         <f>SUM(H3:H121)</f>
-        <v>222000</v>
+        <v>226000</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="16">
         <f>SUM(I2:AM2)</f>
-        <v>222000</v>
+        <v>226000</v>
       </c>
       <c r="I2" s="10">
         <f t="shared" ref="I2:AB2" si="0">SUM(I3:I121)</f>
@@ -4870,7 +4874,7 @@
       </c>
       <c r="N2" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="O2" s="10">
         <f t="shared" si="0"/>
@@ -5212,7 +5216,10 @@
       </c>
       <c r="H11" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4000</v>
+      </c>
+      <c r="N11" s="11">
+        <v>4000</v>
       </c>
       <c r="AB11" s="21"/>
     </row>
@@ -7291,7 +7298,7 @@
       </c>
       <c r="D2" s="6">
         <f>Orders!F2-Collection!H2</f>
-        <v>28500</v>
+        <v>30500</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -7426,7 +7433,7 @@
       </c>
       <c r="D11" s="9">
         <f>Orders!F11-Collection!H11</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
data till 8Mar 8AM
</commit_message>
<xml_diff>
--- a/JioMobile/March2021Mobile.xlsx
+++ b/JioMobile/March2021Mobile.xlsx
@@ -659,11 +659,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -682,8 +682,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -696,22 +697,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -726,26 +721,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -754,37 +747,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -805,9 +767,47 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -826,12 +826,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -906,7 +906,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -924,49 +1026,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -978,109 +1074,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1109,25 +1109,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1150,11 +1137,39 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1170,21 +1185,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1211,7 +1211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1229,130 +1229,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7262,7 +7262,7 @@
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D59" sqref="A1:D59"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
data till 30Mar 8AM
</commit_message>
<xml_diff>
--- a/JioMobile/March2021Mobile.xlsx
+++ b/JioMobile/March2021Mobile.xlsx
@@ -305,6 +305,29 @@
         </r>
       </text>
     </comment>
+    <comment ref="AK80" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Sold 1 mobile to Kedar
+for Rs 1650</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="U88" authorId="0">
       <text>
         <r>
@@ -871,11 +894,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -895,8 +918,68 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -918,14 +1001,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -934,15 +1009,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -955,95 +1061,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -1124,19 +1147,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1154,37 +1249,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1196,13 +1273,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1214,73 +1297,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1323,11 +1346,39 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1362,50 +1413,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1423,13 +1446,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1441,127 +1464,127 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2015,11 +2038,11 @@
   <dimension ref="A1:AT114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="AD53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="AK74" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AF72" sqref="AF72"/>
+      <selection pane="bottomRight" activeCell="AL80" sqref="AL80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2167,26 +2190,26 @@
       <c r="A2" s="13"/>
       <c r="B2" s="24">
         <f>SUM(F3:F121)</f>
-        <v>321000</v>
+        <v>325500</v>
       </c>
       <c r="D2" s="14">
         <f>SUM(H3:H121)</f>
-        <v>321000</v>
+        <v>325500</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="25">
         <f>H2+I2</f>
-        <v>321000</v>
+        <v>325500</v>
       </c>
       <c r="G2" s="25">
         <f>H2/1500</f>
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H2" s="14">
         <f>SUM(J2:AN2)</f>
-        <v>321000</v>
+        <v>325500</v>
       </c>
       <c r="I2" s="32">
         <f>SUM(I3:I121)</f>
@@ -2302,11 +2325,11 @@
       </c>
       <c r="AK2" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="AL2" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="AM2" s="10">
         <f t="shared" si="0"/>
@@ -4424,7 +4447,7 @@
       </c>
       <c r="I79" s="33"/>
     </row>
-    <row r="80" s="11" customFormat="1" spans="1:27">
+    <row r="80" s="11" customFormat="1" spans="1:38">
       <c r="A80" s="11">
         <v>78</v>
       </c>
@@ -4434,15 +4457,15 @@
       </c>
       <c r="F80" s="10">
         <f t="shared" si="7"/>
-        <v>15000</v>
+        <v>16500</v>
       </c>
       <c r="G80" s="10">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H80" s="10">
         <f t="shared" si="9"/>
-        <v>15000</v>
+        <v>16500</v>
       </c>
       <c r="I80" s="33"/>
       <c r="J80" s="29"/>
@@ -4477,6 +4500,10 @@
         <v>1500</v>
       </c>
       <c r="AA80" s="11">
+        <f>1*1500</f>
+        <v>1500</v>
+      </c>
+      <c r="AL80" s="11">
         <f>1*1500</f>
         <v>1500</v>
       </c>
@@ -4803,7 +4830,7 @@
       <c r="X91" s="34"/>
       <c r="Y91" s="34"/>
     </row>
-    <row r="92" s="11" customFormat="1" spans="1:27">
+    <row r="92" s="11" customFormat="1" spans="1:37">
       <c r="A92" s="11">
         <v>90</v>
       </c>
@@ -4812,18 +4839,22 @@
       </c>
       <c r="F92" s="10">
         <f t="shared" si="7"/>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="G92" s="10">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H92" s="10">
         <f t="shared" si="9"/>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="I92" s="33"/>
       <c r="AA92" s="11">
+        <f>2*1500</f>
+        <v>3000</v>
+      </c>
+      <c r="AK92" s="11">
         <f>2*1500</f>
         <v>3000</v>
       </c>
@@ -4982,11 +5013,11 @@
   <dimension ref="A1:AM112"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="Y3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="AF79" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
+      <selection pane="bottomRight" activeCell="AK80" sqref="AK80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -5134,14 +5165,14 @@
       <c r="E2" s="13"/>
       <c r="F2" s="14">
         <f>SUM(H3:H121)</f>
-        <v>308500</v>
+        <v>313000</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="16">
         <f>SUM(I2:AM2)</f>
-        <v>308500</v>
+        <v>313000</v>
       </c>
       <c r="I2" s="10">
         <f t="shared" ref="I2:AB2" si="0">SUM(I3:I121)</f>
@@ -5253,11 +5284,11 @@
       </c>
       <c r="AJ2" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="AK2" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="AL2" s="10">
         <f t="shared" si="1"/>
@@ -7208,7 +7239,7 @@
       </c>
       <c r="AB79" s="21"/>
     </row>
-    <row r="80" s="11" customFormat="1" spans="1:28">
+    <row r="80" s="11" customFormat="1" spans="1:37">
       <c r="A80" s="11">
         <v>78</v>
       </c>
@@ -7220,7 +7251,7 @@
       </c>
       <c r="H80" s="10">
         <f t="shared" si="4"/>
-        <v>15000</v>
+        <v>16500</v>
       </c>
       <c r="P80" s="11">
         <v>1500</v>
@@ -7241,6 +7272,9 @@
         <v>1500</v>
       </c>
       <c r="AB80" s="21"/>
+      <c r="AK80" s="11">
+        <v>1500</v>
+      </c>
     </row>
     <row r="81" s="11" customFormat="1" spans="1:28">
       <c r="A81" s="11">
@@ -7472,7 +7506,7 @@
       </c>
       <c r="AB91" s="21"/>
     </row>
-    <row r="92" s="11" customFormat="1" spans="1:28">
+    <row r="92" s="11" customFormat="1" spans="1:36">
       <c r="A92" s="11">
         <v>90</v>
       </c>
@@ -7490,12 +7524,15 @@
       </c>
       <c r="H92" s="10">
         <f t="shared" si="4"/>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="Z92" s="11">
         <v>3000</v>
       </c>
       <c r="AB92" s="21"/>
+      <c r="AJ92" s="19">
+        <v>3000</v>
+      </c>
     </row>
     <row r="93" s="11" customFormat="1" spans="1:28">
       <c r="A93" s="11">
@@ -7625,7 +7662,7 @@
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D59" sqref="A1:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>

</xml_diff>